<commit_message>
fix testdata to make zettle tests work
</commit_message>
<xml_diff>
--- a/src/testdata/Zettle-Receipts-Report-20210101-20210910.xlsx
+++ b/src/testdata/Zettle-Receipts-Report-20210101-20210910.xlsx
@@ -85,12 +85,12 @@
     <t xml:space="preserve">Betalingsmetode</t>
   </si>
   <si>
+    <t xml:space="preserve">Hændelsestype</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kortudsteder</t>
   </si>
   <si>
-    <t xml:space="preserve">Hændelsestype</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sidste cifre</t>
   </si>
   <si>
@@ -106,10 +106,10 @@
     <t xml:space="preserve">Contactless</t>
   </si>
   <si>
+    <t xml:space="preserve">Køb</t>
+  </si>
+  <si>
     <t xml:space="preserve">VISA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Køb</t>
   </si>
   <si>
     <t xml:space="preserve">BornHack Bar</t>
@@ -296,7 +296,7 @@
   <dimension ref="A2:N26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -305,12 +305,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="25.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="66.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.29"/>
@@ -540,10 +541,10 @@
         <v>27</v>
       </c>
       <c r="I19" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="K19" s="0" t="n">
         <v>2345</v>
@@ -671,8 +672,8 @@
       <c r="H22" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="J22" s="0" t="s">
-        <v>29</v>
+      <c r="I22" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="L22" s="0" t="s">
         <v>34</v>
@@ -709,8 +710,8 @@
       <c r="H23" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="J23" s="0" t="s">
-        <v>29</v>
+      <c r="I23" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="L23" s="0" t="s">
         <v>34</v>

</xml_diff>